<commit_message>
New test resources to fix tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test-create-1.xlsx
+++ b/src/test/resources/test-create-1.xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0" showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView tabRatio="500" windowHeight="19020" windowWidth="25600" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -56,16 +56,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -74,10 +74,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -231,7 +231,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -240,13 +240,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -256,7 +256,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -265,7 +265,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -274,7 +274,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -284,12 +284,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -320,7 +320,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -339,7 +339,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -390,8 +390,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -405,7 +405,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>